<commit_message>
modify part1's rf: adjust rf to the same period of return (we used annual rf in all circumstances in the past, which was not correct)
</commit_message>
<xml_diff>
--- a/output/part1/grs_size_bm.xlsx
+++ b/output/part1/grs_size_bm.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.224993165299287</v>
+        <v>11.57859689929607</v>
       </c>
       <c r="C2" t="n">
         <v>1.110223024625157e-16</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09858588808612984</v>
+        <v>0.006584762722779137</v>
       </c>
       <c r="E2" t="n">
-        <v>-20.87236903279183</v>
+        <v>1.155687290788629</v>
       </c>
       <c r="F2" t="n">
-        <v>435.6557890410472</v>
+        <v>1.33561311409036</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.079020042302525</v>
+        <v>11.5818716894209</v>
       </c>
       <c r="C3" t="n">
         <v>1.110223024625157e-16</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0959201258725121</v>
+        <v>0.006592622778624523</v>
       </c>
       <c r="E3" t="n">
-        <v>-20.30798021653761</v>
+        <v>1.157066803920359</v>
       </c>
       <c r="F3" t="n">
-        <v>412.414060475283</v>
+        <v>1.338803588734474</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.101663364802431</v>
+        <v>11.66686526031629</v>
       </c>
       <c r="C4" t="n">
         <v>1.110223024625157e-16</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09814453814710244</v>
+        <v>0.006561885581899966</v>
       </c>
       <c r="E4" t="n">
-        <v>-20.77892747661361</v>
+        <v>1.151672139130669</v>
       </c>
       <c r="F4" t="n">
-        <v>431.7638270783679</v>
+        <v>1.32634871604981</v>
       </c>
     </row>
     <row r="5">
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.820461166813346</v>
+        <v>11.31480373257072</v>
       </c>
       <c r="C5" t="n">
         <v>1.110223024625157e-16</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09081915688691866</v>
+        <v>0.006888146577582315</v>
       </c>
       <c r="E5" t="n">
-        <v>-19.22801523210581</v>
+        <v>1.208933987744554</v>
       </c>
       <c r="F5" t="n">
-        <v>369.7165697660932</v>
+        <v>1.46152138672395</v>
       </c>
     </row>
     <row r="6">
@@ -555,19 +555,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.976048224525601</v>
+        <v>11.67864002591413</v>
       </c>
       <c r="C6" t="n">
         <v>1.110223024625157e-16</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09562872657523547</v>
+        <v>0.006567999196042228</v>
       </c>
       <c r="E6" t="n">
-        <v>-20.24628585249901</v>
+        <v>1.152745135449968</v>
       </c>
       <c r="F6" t="n">
-        <v>409.9120908211017</v>
+        <v>1.328821347303564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>